<commit_message>
17.06.13 12:03 - Logic edited
</commit_message>
<xml_diff>
--- a/HW-2/Documentation/Баланс.xlsx
+++ b/HW-2/Documentation/Баланс.xlsx
@@ -409,9 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>